<commit_message>
Update DATA SISWA  - PERUSAHAAN.xlsx
</commit_message>
<xml_diff>
--- a/temp_doc/DATA SISWA  - PERUSAHAAN.xlsx
+++ b/temp_doc/DATA SISWA  - PERUSAHAAN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\bkk\temp_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E73DC0-E84D-405D-82CC-A6FBDFDF839B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1743DE-2F88-49A1-B918-6B9C6E35F4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{A22911EF-5D24-2343-8839-FFE0F546D574}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{A22911EF-5D24-2343-8839-FFE0F546D574}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17439" uniqueCount="2972">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17443" uniqueCount="2974">
   <si>
     <t>id</t>
   </si>
@@ -9031,11 +9031,20 @@
   <si>
     <t>SISA</t>
   </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -9070,12 +9079,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -9105,11 +9120,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -36541,10 +36566,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B15449E-4AD6-49F4-8245-C2C6100A2151}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -36554,16 +36579,17 @@
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.75" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" customWidth="1"/>
-    <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.125" customWidth="1"/>
-    <col min="16" max="16" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.25" customWidth="1"/>
+    <col min="13" max="13" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2960</v>
       </c>
@@ -36583,25 +36609,31 @@
         <v>2964</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>2970</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>2971</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>2965</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>2966</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>2967</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>2968</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>2970</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>2971</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2022</v>
       </c>
@@ -36624,21 +36656,33 @@
       <c r="I2" s="1" t="s">
         <v>2960</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1">
+        <v>64</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
+      <c r="M2" s="1">
+        <v>7</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
       <c r="O2" s="1">
-        <f>SUM(J2:M2)</f>
+        <v>2</v>
+      </c>
+      <c r="P2" s="1">
+        <v>74</v>
+      </c>
+      <c r="Q2" s="1">
+        <f>SUM(J2:O2)</f>
+        <v>74</v>
+      </c>
+      <c r="R2" s="1">
+        <f>P2-Q2</f>
         <v>0</v>
       </c>
-      <c r="P2" s="1">
-        <f>N2-O2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -36661,54 +36705,147 @@
       <c r="I3" s="1" t="s">
         <v>2961</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1">
+        <v>57</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+      <c r="M3" s="1">
+        <v>5</v>
+      </c>
+      <c r="N3" s="1">
+        <v>4</v>
+      </c>
       <c r="O3" s="1">
-        <f t="shared" ref="O3:O5" si="0">SUM(J3:M3)</f>
+        <v>3</v>
+      </c>
+      <c r="P3" s="1">
+        <v>69</v>
+      </c>
+      <c r="Q3" s="1">
+        <f>SUM(J3:O3)</f>
+        <v>69</v>
+      </c>
+      <c r="R3" s="1">
+        <f t="shared" ref="R3:R5" si="0">P3-Q3</f>
         <v>0</v>
       </c>
-      <c r="P3" s="1">
-        <f t="shared" ref="P3:P5" si="1">N3-O3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I4" s="1" t="s">
         <v>2962</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="1">
+        <v>69</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
+      <c r="M4" s="1">
+        <v>6</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
       <c r="O4" s="1">
+        <v>4</v>
+      </c>
+      <c r="P4" s="1">
+        <v>80</v>
+      </c>
+      <c r="Q4" s="1">
+        <f>SUM(J4:O4)</f>
+        <v>80</v>
+      </c>
+      <c r="R4" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P4" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I5" s="1" t="s">
         <v>2963</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1">
+        <v>98</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+      <c r="M5" s="1">
+        <v>5</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
       <c r="O5" s="1">
+        <v>4</v>
+      </c>
+      <c r="P5" s="1">
+        <v>108</v>
+      </c>
+      <c r="Q5" s="1">
+        <f>SUM(J5:O5)</f>
+        <v>108</v>
+      </c>
+      <c r="R5" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P5" s="1">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I6" s="2"/>
+      <c r="J6" s="5">
+        <f>(SUM(J2:J5))</f>
+        <v>288</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5">
+        <f t="shared" ref="M6:O6" si="1">(SUM(M2:M5))</f>
+        <v>23</v>
+      </c>
+      <c r="N6" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="O6" s="5">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="P6" s="2">
+        <f>SUM(P2:P5)</f>
+        <v>331</v>
+      </c>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M10" s="3"/>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M11" s="3"/>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M12" s="3"/>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M13" s="3"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M14" s="3"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="21" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
+        <v>2972</v>
       </c>
     </row>
   </sheetData>
@@ -36723,7 +36860,7 @@
   <dimension ref="A1:O126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -36796,7 +36933,7 @@
       <c r="A2">
         <v>10001</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>102</v>
       </c>
       <c r="C2" t="s">
@@ -36843,7 +36980,7 @@
       <c r="A3">
         <v>10002</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>106</v>
       </c>
       <c r="C3" t="s">
@@ -42688,8 +42825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DABFED43-A481-4D87-98FF-2069F4EC1CB0}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -42758,144 +42895,144 @@
         <v>2959</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
         <v>10001</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="7">
         <v>89652561486</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2">
+      <c r="G2" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="7">
         <v>2022</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="7" t="s">
         <v>2192</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="7" t="s">
         <v>2322</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="7" t="s">
         <v>2501</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="7" t="s">
         <v>2323</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="7" t="s">
         <v>2635</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="7" t="s">
         <v>2501</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="7" t="s">
         <v>2785</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>10002</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="G3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H3">
+      <c r="G3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="7">
         <v>2022</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="7" t="s">
         <v>2193</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="7" t="s">
         <v>2324</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="7" t="s">
         <v>2502</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="7" t="s">
         <v>2323</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="7" t="s">
         <v>2636</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="7" t="s">
         <v>2502</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="7" t="s">
         <v>2786</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>10003</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4">
+      <c r="G4" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="7">
         <v>2022</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="7" t="s">
         <v>2194</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="7" t="s">
         <v>2325</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="7" t="s">
         <v>2503</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="7" t="s">
         <v>2323</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="7" t="s">
         <v>2637</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="7" t="s">
         <v>2503</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="7" t="s">
         <v>2785</v>
       </c>
     </row>
@@ -43416,10 +43553,13 @@
         <v>2786</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>COUNTA(B2:B15)</f>
         <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>